<commit_message>
Finished input file scripts for ref scenario
</commit_message>
<xml_diff>
--- a/HydroFPV_plants/CombinedTechsCreation/CombinedHydroSolar.xlsx
+++ b/HydroFPV_plants/CombinedTechsCreation/CombinedHydroSolar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro Pieruzzi\Documents\Thesis\TEMBA_FPV\HydroFPV_plants\CombinedTechsCreation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1903BF4D-9FF6-427D-94A2-7D20D39610EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8A1CBE-15BE-4B72-840F-67A50ECA770B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="74">
   <si>
     <t>Country</t>
   </si>
@@ -661,7 +661,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1724,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FC710B-81A7-4A19-B13B-3AD951BA7D4B}">
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1752,7 +1752,7 @@
     <col min="23" max="23" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1822,8 +1822,11 @@
       <c r="W1" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1894,8 +1897,11 @@
       <c r="W2">
         <v>0.1117774126984127</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1965,8 +1971,11 @@
       <c r="W3">
         <v>0.1126826774193548</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2036,8 +2045,11 @@
       <c r="W4">
         <v>0.1126826774193548</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X4">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2107,8 +2119,11 @@
       <c r="W5">
         <v>0.11339636354326681</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2176,8 +2191,11 @@
       <c r="W6">
         <v>0.111860513312852</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X6">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2244,8 +2262,11 @@
       <c r="W7">
         <v>0.13024408422939071</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X7">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2313,8 +2334,11 @@
       <c r="W8">
         <v>0.1242511758832565</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X8">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2381,8 +2405,11 @@
       <c r="W9">
         <v>9.809929006656426E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X9">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2434,7 +2461,7 @@
         <v>0.14075010650281619</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2505,8 +2532,11 @@
       <c r="W11">
         <v>0.1216317309267793</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X11">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2576,8 +2606,11 @@
       <c r="W12">
         <v>0.11319275345622121</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X12">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2647,8 +2680,11 @@
       <c r="W13">
         <v>0.1173318461341526</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X13">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -2719,8 +2755,11 @@
       <c r="W14">
         <v>0.1194960299539171</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X14">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2787,8 +2826,11 @@
       <c r="W15">
         <v>0.1130760087045571</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X15">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2856,8 +2898,11 @@
       <c r="W16">
         <v>0.12482191730670759</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X16">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2924,8 +2969,11 @@
       <c r="W17">
         <v>0.1174430401945725</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X17">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2992,8 +3040,11 @@
       <c r="W18">
         <v>0.12382463159242189</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X18">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -3061,8 +3112,11 @@
       <c r="W19">
         <v>0.12471186533538151</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X19">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -3129,8 +3183,11 @@
       <c r="W20">
         <v>0.124365051203277</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X20">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>7</v>
       </c>
@@ -3173,8 +3230,11 @@
       <c r="U21" s="12">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X21">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>7</v>
       </c>
@@ -3217,8 +3277,11 @@
       <c r="U22" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X22">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
@@ -3261,8 +3324,11 @@
       <c r="U23" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X23">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>17</v>
       </c>
@@ -3305,8 +3371,11 @@
       <c r="U24" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X24">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>17</v>
       </c>
@@ -3349,11 +3418,11 @@
       <c r="U25" s="12">
         <v>1</v>
       </c>
+      <c r="X25">
+        <v>2000</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:G25">
-    <sortCondition ref="A21:A25"/>
-  </sortState>
   <conditionalFormatting sqref="G2:G20">
     <cfRule type="colorScale" priority="89">
       <colorScale>

</xml_diff>

<commit_message>
many updates I forgot
</commit_message>
<xml_diff>
--- a/HydroFPV_plants/CombinedTechsCreation/CombinedHydroSolar.xlsx
+++ b/HydroFPV_plants/CombinedTechsCreation/CombinedHydroSolar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro Pieruzzi\Documents\Thesis\TEMBA_FPV\HydroFPV_plants\CombinedTechsCreation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E80FB86C-A85C-4E87-B1C1-4A9B1A5EC9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97F2C03-7D91-4527-95B9-F130F7FE9147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CombinedHydroSolar" sheetId="1" r:id="rId1"/>
@@ -2098,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12D4CD1-EA60-45BC-AF7D-FB8E106958A4}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5805,8 +5805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8015D18A-6D36-49CD-83E7-E734D0F41EA6}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6980,23 +6980,47 @@
       <c r="K15">
         <v>550</v>
       </c>
+      <c r="L15">
+        <v>0.5</v>
+      </c>
+      <c r="M15">
+        <v>0.5</v>
+      </c>
       <c r="N15">
         <v>0.32026751971326162</v>
       </c>
       <c r="O15">
         <v>0.1044625844683393</v>
       </c>
+      <c r="P15">
+        <v>0.5</v>
+      </c>
+      <c r="Q15">
+        <v>0.5</v>
+      </c>
       <c r="R15">
         <v>0.26110407606531272</v>
       </c>
       <c r="S15">
         <v>7.1898174910394255E-2</v>
       </c>
+      <c r="T15">
+        <v>0.5</v>
+      </c>
+      <c r="U15">
+        <v>0.5</v>
+      </c>
       <c r="V15">
         <v>0.31357061529271207</v>
       </c>
       <c r="W15">
         <v>0.1066021416965352</v>
+      </c>
+      <c r="X15">
+        <v>0.5</v>
+      </c>
+      <c r="Y15">
+        <v>0.5</v>
       </c>
       <c r="Z15">
         <v>0.3784216705069125</v>
@@ -13195,7 +13219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4077C91D-7F68-4E04-B52C-E724C959D063}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Crazy last minute changes
</commit_message>
<xml_diff>
--- a/HydroFPV_plants/CombinedTechsCreation/CombinedHydroSolar.xlsx
+++ b/HydroFPV_plants/CombinedTechsCreation/CombinedHydroSolar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro Pieruzzi\Documents\Thesis\TEMBA_FPV\HydroFPV_plants\CombinedTechsCreation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97F2C03-7D91-4527-95B9-F130F7FE9147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD4D56D-DE71-4E43-9449-70826894B054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CombinedHydroSolar" sheetId="1" r:id="rId1"/>
@@ -5805,7 +5805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8015D18A-6D36-49CD-83E7-E734D0F41EA6}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -18428,8 +18428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FC710B-81A7-4A19-B13B-3AD951BA7D4B}">
   <dimension ref="A1:AC49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22:F49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18440,7 +18440,7 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
     <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="14.140625" customWidth="1"/>

</xml_diff>